<commit_message>
Occupations encore et encore et toujours
</commit_message>
<xml_diff>
--- a/Occupations/Occupations.xlsx
+++ b/Occupations/Occupations.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252041" uniqueCount="1314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255062" uniqueCount="1314">
   <si>
     <t>occupationname</t>
   </si>
@@ -31127,10 +31127,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B4" t="s">
-        <v>773</v>
+        <v>48</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" t="s">
@@ -31145,10 +31145,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>773</v>
       </c>
       <c r="C5" s="0"/>
       <c r="D5" t="s">
@@ -31163,10 +31163,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B6" t="s">
-        <v>1184</v>
+        <v>309</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" t="s">
@@ -31179,10 +31179,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>1184</v>
       </c>
       <c r="C7" s="0"/>
       <c r="D7" t="s">
@@ -31273,10 +31273,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>775</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" t="s">
@@ -31291,10 +31291,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B14" t="s">
-        <v>775</v>
+        <v>262</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" t="s">
@@ -31312,7 +31312,7 @@
         <v>748</v>
       </c>
       <c r="B15" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C15" s="0"/>
       <c r="D15" t="s">
@@ -31501,10 +31501,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B26" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C26" s="0"/>
       <c r="D26" t="s">
@@ -31519,10 +31519,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B27" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" t="s">
@@ -31675,10 +31675,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B36" t="s">
-        <v>775</v>
+        <v>463</v>
       </c>
       <c r="C36" s="0"/>
       <c r="D36" t="s">
@@ -31693,10 +31693,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B37" t="s">
-        <v>463</v>
+        <v>775</v>
       </c>
       <c r="C37" s="0"/>
       <c r="D37" t="s">
@@ -31852,7 +31852,7 @@
         <v>748</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>286</v>
       </c>
       <c r="C46" s="0"/>
       <c r="D46" t="s">
@@ -31866,7 +31866,7 @@
         <v>748</v>
       </c>
       <c r="B47" t="s">
-        <v>286</v>
+        <v>48</v>
       </c>
       <c r="C47" s="0"/>
       <c r="D47" t="s">
@@ -31877,10 +31877,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>752</v>
+        <v>1181</v>
       </c>
       <c r="B48" t="s">
-        <v>309</v>
+        <v>1185</v>
       </c>
       <c r="C48" s="0"/>
       <c r="D48" t="s">
@@ -31891,10 +31891,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>1181</v>
+        <v>752</v>
       </c>
       <c r="B49" t="s">
-        <v>1185</v>
+        <v>309</v>
       </c>
       <c r="C49" s="0"/>
       <c r="D49" t="s">
@@ -31937,10 +31937,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>749</v>
+        <v>1181</v>
       </c>
       <c r="B52" t="s">
-        <v>790</v>
+        <v>1188</v>
       </c>
       <c r="C52" s="0"/>
       <c r="D52" t="s">
@@ -31953,10 +31953,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>1181</v>
+        <v>749</v>
       </c>
       <c r="B53" t="s">
-        <v>1188</v>
+        <v>790</v>
       </c>
       <c r="C53" s="0"/>
       <c r="D53" t="s">
@@ -32018,7 +32018,7 @@
         <v>750</v>
       </c>
       <c r="B57" t="s">
-        <v>486</v>
+        <v>789</v>
       </c>
       <c r="C57" s="0"/>
       <c r="D57" t="s">
@@ -32036,7 +32036,7 @@
         <v>750</v>
       </c>
       <c r="B58" t="s">
-        <v>789</v>
+        <v>486</v>
       </c>
       <c r="C58" s="0"/>
       <c r="D58" t="s">
@@ -32126,7 +32126,7 @@
         <v>1181</v>
       </c>
       <c r="B63" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C63" s="0"/>
       <c r="D63" t="s">
@@ -32144,7 +32144,7 @@
         <v>1181</v>
       </c>
       <c r="B64" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C64" s="0"/>
       <c r="D64" t="s">
@@ -32525,10 +32525,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B86" t="s">
-        <v>624</v>
+        <v>804</v>
       </c>
       <c r="C86" s="0"/>
       <c r="D86" t="s">
@@ -32543,10 +32543,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B87" t="s">
-        <v>804</v>
+        <v>624</v>
       </c>
       <c r="C87" s="0"/>
       <c r="D87" t="s">
@@ -32580,7 +32580,7 @@
         <v>748</v>
       </c>
       <c r="B89" t="s">
-        <v>280</v>
+        <v>804</v>
       </c>
       <c r="C89" s="0"/>
       <c r="D89" t="s">
@@ -32596,7 +32596,7 @@
         <v>748</v>
       </c>
       <c r="B90" t="s">
-        <v>804</v>
+        <v>280</v>
       </c>
       <c r="C90" s="0"/>
       <c r="D90" t="s">
@@ -32943,10 +32943,10 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>748</v>
+        <v>1181</v>
       </c>
       <c r="B111" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C111" s="0"/>
       <c r="D111" t="s">
@@ -32959,10 +32959,10 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>1181</v>
+        <v>748</v>
       </c>
       <c r="B112" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C112" s="0"/>
       <c r="D112" t="s">
@@ -33095,10 +33095,10 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B120" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C120" s="0"/>
       <c r="D120" t="s">
@@ -33113,10 +33113,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B121" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="C121" s="0"/>
       <c r="D121" t="s">
@@ -33239,10 +33239,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B128" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="C128" s="0"/>
       <c r="D128" t="s">
@@ -33255,10 +33255,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B129" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C129" s="0"/>
       <c r="D129" t="s">
@@ -33326,7 +33326,7 @@
         <v>750</v>
       </c>
       <c r="B133" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="C133" s="0"/>
       <c r="D133" t="s">
@@ -33344,7 +33344,7 @@
         <v>750</v>
       </c>
       <c r="B134" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c r="C134" s="0"/>
       <c r="D134" t="s">
@@ -33362,7 +33362,7 @@
         <v>750</v>
       </c>
       <c r="B135" t="s">
-        <v>486</v>
+        <v>336</v>
       </c>
       <c r="C135" s="0"/>
       <c r="D135" t="s">
@@ -33378,7 +33378,7 @@
         <v>750</v>
       </c>
       <c r="B136" t="s">
-        <v>336</v>
+        <v>486</v>
       </c>
       <c r="C136" s="0"/>
       <c r="D136" t="s">
@@ -33394,7 +33394,7 @@
         <v>748</v>
       </c>
       <c r="B137" t="s">
-        <v>336</v>
+        <v>262</v>
       </c>
       <c r="C137" s="0"/>
       <c r="D137" t="s">
@@ -33410,7 +33410,7 @@
         <v>748</v>
       </c>
       <c r="B138" t="s">
-        <v>262</v>
+        <v>336</v>
       </c>
       <c r="C138" s="0"/>
       <c r="D138" t="s">
@@ -33737,10 +33737,10 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B158" t="s">
-        <v>791</v>
+        <v>300</v>
       </c>
       <c r="C158" s="0"/>
       <c r="D158" t="s">
@@ -33755,10 +33755,10 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B159" t="s">
-        <v>300</v>
+        <v>791</v>
       </c>
       <c r="C159" s="0"/>
       <c r="D159" t="s">
@@ -34089,10 +34089,10 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B179" t="s">
-        <v>775</v>
+        <v>791</v>
       </c>
       <c r="C179" s="0"/>
       <c r="D179" t="s">
@@ -34107,10 +34107,10 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B180" t="s">
-        <v>791</v>
+        <v>775</v>
       </c>
       <c r="C180" s="0"/>
       <c r="D180" t="s">
@@ -34313,10 +34313,10 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B192" t="s">
-        <v>1198</v>
+        <v>536</v>
       </c>
       <c r="C192" s="0"/>
       <c r="D192" t="s">
@@ -34329,10 +34329,10 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B193" t="s">
-        <v>536</v>
+        <v>1198</v>
       </c>
       <c r="C193" s="0"/>
       <c r="D193" t="s">
@@ -34345,10 +34345,10 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>752</v>
+        <v>1181</v>
       </c>
       <c r="B194" t="s">
-        <v>1199</v>
+        <v>343</v>
       </c>
       <c r="C194" s="0"/>
       <c r="D194" t="s">
@@ -34361,10 +34361,10 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>1181</v>
+        <v>752</v>
       </c>
       <c r="B195" t="s">
-        <v>343</v>
+        <v>1199</v>
       </c>
       <c r="C195" s="0"/>
       <c r="D195" t="s">
@@ -34479,10 +34479,10 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B202" t="s">
-        <v>262</v>
+        <v>789</v>
       </c>
       <c r="C202" s="0"/>
       <c r="D202" t="s">
@@ -34497,10 +34497,10 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B203" t="s">
-        <v>789</v>
+        <v>262</v>
       </c>
       <c r="C203" s="0"/>
       <c r="D203" t="s">
@@ -34613,10 +34613,10 @@
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>749</v>
+        <v>1181</v>
       </c>
       <c r="B210" t="s">
-        <v>790</v>
+        <v>846</v>
       </c>
       <c r="C210" s="0"/>
       <c r="D210" t="s">
@@ -34631,10 +34631,10 @@
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>1181</v>
+        <v>749</v>
       </c>
       <c r="B211" t="s">
-        <v>846</v>
+        <v>790</v>
       </c>
       <c r="C211" s="0"/>
       <c r="D211" t="s">
@@ -34733,10 +34733,10 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B217" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C217" s="0"/>
       <c r="D217" t="s">
@@ -34749,10 +34749,10 @@
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B218" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C218" s="0"/>
       <c r="D218" t="s">
@@ -34781,10 +34781,10 @@
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B220" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C220" s="0"/>
       <c r="D220" t="s">
@@ -34799,10 +34799,10 @@
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B221" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="C221" s="0"/>
       <c r="D221" t="s">
@@ -34937,10 +34937,10 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B229" t="s">
-        <v>780</v>
+        <v>820</v>
       </c>
       <c r="C229" s="0"/>
       <c r="D229" t="s">
@@ -34953,10 +34953,10 @@
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B230" t="s">
-        <v>820</v>
+        <v>780</v>
       </c>
       <c r="C230" s="0"/>
       <c r="D230" t="s">
@@ -35150,7 +35150,7 @@
         <v>748</v>
       </c>
       <c r="B242" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C242" s="0"/>
       <c r="D242" t="s">
@@ -35166,7 +35166,7 @@
         <v>748</v>
       </c>
       <c r="B243" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C243" s="0"/>
       <c r="D243" t="s">
@@ -35419,10 +35419,10 @@
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B258" t="s">
-        <v>786</v>
+        <v>860</v>
       </c>
       <c r="C258" s="0"/>
       <c r="D258" t="s">
@@ -35437,10 +35437,10 @@
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B259" t="s">
-        <v>860</v>
+        <v>786</v>
       </c>
       <c r="C259" s="0"/>
       <c r="D259" t="s">
@@ -35455,10 +35455,10 @@
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B260" t="s">
-        <v>860</v>
+        <v>786</v>
       </c>
       <c r="C260" s="0"/>
       <c r="D260" t="s">
@@ -35471,10 +35471,10 @@
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B261" t="s">
-        <v>786</v>
+        <v>860</v>
       </c>
       <c r="C261" s="0"/>
       <c r="D261" t="s">
@@ -35587,10 +35587,10 @@
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B268" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C268" s="0"/>
       <c r="D268" t="s">
@@ -35603,10 +35603,10 @@
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B269" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="C269" s="0"/>
       <c r="D269" t="s">
@@ -35767,10 +35767,10 @@
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B279" t="s">
-        <v>535</v>
+        <v>867</v>
       </c>
       <c r="C279" s="0"/>
       <c r="D279" t="s">
@@ -35785,10 +35785,10 @@
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B280" t="s">
-        <v>867</v>
+        <v>535</v>
       </c>
       <c r="C280" s="0"/>
       <c r="D280" t="s">
@@ -36079,10 +36079,10 @@
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>1181</v>
+        <v>748</v>
       </c>
       <c r="B297" t="s">
-        <v>875</v>
+        <v>823</v>
       </c>
       <c r="C297" s="0"/>
       <c r="D297" t="s">
@@ -36097,10 +36097,10 @@
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>748</v>
+        <v>1181</v>
       </c>
       <c r="B298" t="s">
-        <v>823</v>
+        <v>875</v>
       </c>
       <c r="C298" s="0"/>
       <c r="D298" t="s">
@@ -36267,10 +36267,10 @@
     </row>
     <row r="308">
       <c r="A308" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="B308" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C308" s="0"/>
       <c r="D308" t="s">
@@ -36285,10 +36285,10 @@
     </row>
     <row r="309">
       <c r="A309" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="B309" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C309" s="0"/>
       <c r="D309" t="s">
@@ -37068,7 +37068,7 @@
         <v>748</v>
       </c>
       <c r="B355" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C355" s="0"/>
       <c r="D355" t="s">
@@ -37084,7 +37084,7 @@
         <v>748</v>
       </c>
       <c r="B356" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C356" s="0"/>
       <c r="D356" t="s">
@@ -37371,10 +37371,10 @@
     </row>
     <row r="373">
       <c r="A373" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="B373" t="s">
-        <v>278</v>
+        <v>904</v>
       </c>
       <c r="C373" s="0"/>
       <c r="D373" t="s">
@@ -37389,10 +37389,10 @@
     </row>
     <row r="374">
       <c r="A374" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="B374" t="s">
-        <v>904</v>
+        <v>278</v>
       </c>
       <c r="C374" s="0"/>
       <c r="D374" t="s">
@@ -37654,7 +37654,7 @@
         <v>748</v>
       </c>
       <c r="B389" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C389" s="0"/>
       <c r="D389" t="s">
@@ -37670,7 +37670,7 @@
         <v>748</v>
       </c>
       <c r="B390" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C390" s="0"/>
       <c r="D390" t="s">
@@ -37686,7 +37686,7 @@
         <v>748</v>
       </c>
       <c r="B391" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C391" s="0"/>
       <c r="D391" t="s">
@@ -38373,10 +38373,10 @@
     </row>
     <row r="432">
       <c r="A432" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B432" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C432" s="0"/>
       <c r="D432" t="s">
@@ -38389,10 +38389,10 @@
     </row>
     <row r="433">
       <c r="A433" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B433" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C433" s="0"/>
       <c r="D433" t="s">
@@ -38442,7 +38442,7 @@
         <v>750</v>
       </c>
       <c r="B436" t="s">
-        <v>932</v>
+        <v>517</v>
       </c>
       <c r="C436" s="0"/>
       <c r="D436" t="s">
@@ -38458,7 +38458,7 @@
         <v>750</v>
       </c>
       <c r="B437" t="s">
-        <v>517</v>
+        <v>932</v>
       </c>
       <c r="C437" s="0"/>
       <c r="D437" t="s">
@@ -38471,10 +38471,10 @@
     </row>
     <row r="438">
       <c r="A438" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B438" t="s">
-        <v>324</v>
+        <v>517</v>
       </c>
       <c r="C438" s="0"/>
       <c r="D438" t="s">
@@ -38489,10 +38489,10 @@
     </row>
     <row r="439">
       <c r="A439" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B439" t="s">
-        <v>517</v>
+        <v>324</v>
       </c>
       <c r="C439" s="0"/>
       <c r="D439" t="s">
@@ -38622,7 +38622,7 @@
         <v>750</v>
       </c>
       <c r="B447" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C447" s="0"/>
       <c r="D447" t="s">
@@ -38658,7 +38658,7 @@
         <v>750</v>
       </c>
       <c r="B449" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C449" s="0"/>
       <c r="D449" t="s">
@@ -38911,10 +38911,10 @@
     </row>
     <row r="464">
       <c r="A464" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B464" t="s">
-        <v>278</v>
+        <v>899</v>
       </c>
       <c r="C464" s="0"/>
       <c r="D464" t="s">
@@ -38929,10 +38929,10 @@
     </row>
     <row r="465">
       <c r="A465" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B465" t="s">
-        <v>899</v>
+        <v>278</v>
       </c>
       <c r="C465" s="0"/>
       <c r="D465" t="s">
@@ -38963,10 +38963,10 @@
     </row>
     <row r="467">
       <c r="A467" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B467" t="s">
-        <v>300</v>
+        <v>1223</v>
       </c>
       <c r="C467" s="0"/>
       <c r="D467" t="s">
@@ -38977,10 +38977,10 @@
     </row>
     <row r="468">
       <c r="A468" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B468" t="s">
-        <v>1223</v>
+        <v>300</v>
       </c>
       <c r="C468" s="0"/>
       <c r="D468" t="s">
@@ -39061,10 +39061,10 @@
     </row>
     <row r="473">
       <c r="A473" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B473" t="s">
-        <v>1224</v>
+        <v>429</v>
       </c>
       <c r="C473" s="0"/>
       <c r="D473" t="s">
@@ -39093,10 +39093,10 @@
     </row>
     <row r="475">
       <c r="A475" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B475" t="s">
-        <v>429</v>
+        <v>1224</v>
       </c>
       <c r="C475" s="0"/>
       <c r="D475" t="s">
@@ -39192,7 +39192,7 @@
         <v>750</v>
       </c>
       <c r="B481" t="s">
-        <v>316</v>
+        <v>946</v>
       </c>
       <c r="C481" s="0"/>
       <c r="D481" t="s">
@@ -39210,7 +39210,7 @@
         <v>750</v>
       </c>
       <c r="B482" t="s">
-        <v>946</v>
+        <v>316</v>
       </c>
       <c r="C482" s="0"/>
       <c r="D482" t="s">
@@ -39246,7 +39246,7 @@
         <v>1181</v>
       </c>
       <c r="B484" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C484" s="0"/>
       <c r="D484" t="s">
@@ -39262,7 +39262,7 @@
         <v>1181</v>
       </c>
       <c r="B485" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="C485" s="0"/>
       <c r="D485" t="s">
@@ -39503,10 +39503,10 @@
     </row>
     <row r="499">
       <c r="A499" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B499" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="C499" s="0"/>
       <c r="D499" t="s">
@@ -39521,10 +39521,10 @@
     </row>
     <row r="500">
       <c r="A500" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B500" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C500" s="0"/>
       <c r="D500" t="s">
@@ -39890,7 +39890,7 @@
         <v>748</v>
       </c>
       <c r="B522" t="s">
-        <v>47</v>
+        <v>804</v>
       </c>
       <c r="C522" s="0"/>
       <c r="D522" t="s">
@@ -39908,7 +39908,7 @@
         <v>748</v>
       </c>
       <c r="B523" t="s">
-        <v>804</v>
+        <v>47</v>
       </c>
       <c r="C523" s="0"/>
       <c r="D523" t="s">
@@ -40131,10 +40131,10 @@
     </row>
     <row r="536">
       <c r="A536" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B536" t="s">
-        <v>967</v>
+        <v>198</v>
       </c>
       <c r="C536" s="0"/>
       <c r="D536" t="s">
@@ -40149,10 +40149,10 @@
     </row>
     <row r="537">
       <c r="A537" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B537" t="s">
-        <v>198</v>
+        <v>967</v>
       </c>
       <c r="C537" s="0"/>
       <c r="D537" t="s">
@@ -40185,10 +40185,10 @@
     </row>
     <row r="539">
       <c r="A539" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B539" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="C539" s="0"/>
       <c r="D539" t="s">
@@ -40201,10 +40201,10 @@
     </row>
     <row r="540">
       <c r="A540" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B540" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C540" s="0"/>
       <c r="D540" t="s">
@@ -41027,10 +41027,10 @@
     </row>
     <row r="589">
       <c r="A589" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B589" t="s">
-        <v>264</v>
+        <v>790</v>
       </c>
       <c r="C589" s="0"/>
       <c r="D589" t="s">
@@ -41043,10 +41043,10 @@
     </row>
     <row r="590">
       <c r="A590" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B590" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C590" s="0"/>
       <c r="D590" t="s">
@@ -41059,10 +41059,10 @@
     </row>
     <row r="591">
       <c r="A591" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B591" t="s">
-        <v>790</v>
+        <v>262</v>
       </c>
       <c r="C591" s="0"/>
       <c r="D591" t="s">
@@ -41394,7 +41394,7 @@
         <v>748</v>
       </c>
       <c r="B610" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C610" s="0"/>
       <c r="D610" t="s">
@@ -41412,7 +41412,7 @@
         <v>748</v>
       </c>
       <c r="B611" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C611" s="0"/>
       <c r="D611" t="s">
@@ -41745,10 +41745,10 @@
     </row>
     <row r="631">
       <c r="A631" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B631" t="s">
-        <v>1012</v>
+        <v>448</v>
       </c>
       <c r="C631" s="0"/>
       <c r="D631" t="s">
@@ -41763,10 +41763,10 @@
     </row>
     <row r="632">
       <c r="A632" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B632" t="s">
-        <v>448</v>
+        <v>1012</v>
       </c>
       <c r="C632" s="0"/>
       <c r="D632" t="s">
@@ -41917,10 +41917,10 @@
     </row>
     <row r="641">
       <c r="A641" t="s">
-        <v>748</v>
+        <v>753</v>
       </c>
       <c r="B641" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C641" s="0"/>
       <c r="D641" t="s">
@@ -41933,10 +41933,10 @@
     </row>
     <row r="642">
       <c r="A642" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="B642" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C642" s="0"/>
       <c r="D642" t="s">
@@ -42123,10 +42123,10 @@
     </row>
     <row r="653">
       <c r="A653" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B653" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="C653" s="0"/>
       <c r="D653" t="s">
@@ -42139,10 +42139,10 @@
     </row>
     <row r="654">
       <c r="A654" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B654" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C654" s="0"/>
       <c r="D654" t="s">
@@ -42503,10 +42503,10 @@
     </row>
     <row r="676">
       <c r="A676" t="s">
-        <v>1181</v>
+        <v>749</v>
       </c>
       <c r="B676" t="s">
-        <v>925</v>
+        <v>273</v>
       </c>
       <c r="C676" s="0"/>
       <c r="D676" t="s">
@@ -42519,10 +42519,10 @@
     </row>
     <row r="677">
       <c r="A677" t="s">
-        <v>749</v>
+        <v>1181</v>
       </c>
       <c r="B677" t="s">
-        <v>273</v>
+        <v>925</v>
       </c>
       <c r="C677" s="0"/>
       <c r="D677" t="s">
@@ -42535,10 +42535,10 @@
     </row>
     <row r="678">
       <c r="A678" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B678" t="s">
-        <v>925</v>
+        <v>273</v>
       </c>
       <c r="C678" s="0"/>
       <c r="D678" t="s">
@@ -42551,10 +42551,10 @@
     </row>
     <row r="679">
       <c r="A679" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="B679" t="s">
-        <v>273</v>
+        <v>925</v>
       </c>
       <c r="C679" s="0"/>
       <c r="D679" t="s">
@@ -42783,10 +42783,10 @@
     </row>
     <row r="693">
       <c r="A693" t="s">
-        <v>748</v>
+        <v>1181</v>
       </c>
       <c r="B693" t="s">
-        <v>689</v>
+        <v>547</v>
       </c>
       <c r="C693" s="0"/>
       <c r="D693" t="s">
@@ -42801,10 +42801,10 @@
     </row>
     <row r="694">
       <c r="A694" t="s">
-        <v>1181</v>
+        <v>748</v>
       </c>
       <c r="B694" t="s">
-        <v>547</v>
+        <v>689</v>
       </c>
       <c r="C694" s="0"/>
       <c r="D694" t="s">
@@ -42954,7 +42954,7 @@
         <v>750</v>
       </c>
       <c r="B703" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="C703" s="0"/>
       <c r="D703" t="s">
@@ -42970,7 +42970,7 @@
         <v>750</v>
       </c>
       <c r="B704" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C704" s="0"/>
       <c r="D704" t="s">
@@ -43347,10 +43347,10 @@
     </row>
     <row r="726">
       <c r="A726" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B726" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C726" s="0"/>
       <c r="D726" t="s">
@@ -43363,10 +43363,10 @@
     </row>
     <row r="727">
       <c r="A727" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B727" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C727" s="0"/>
       <c r="D727" t="s">
@@ -44210,7 +44210,7 @@
         <v>750</v>
       </c>
       <c r="B776" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="C776" s="0"/>
       <c r="D776" t="s">
@@ -44226,7 +44226,7 @@
         <v>750</v>
       </c>
       <c r="B777" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C777" s="0"/>
       <c r="D777" t="s">
@@ -44242,7 +44242,7 @@
         <v>748</v>
       </c>
       <c r="B778" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="C778" s="0"/>
       <c r="D778" t="s">
@@ -44256,7 +44256,7 @@
         <v>748</v>
       </c>
       <c r="B779" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C779" s="0"/>
       <c r="D779" t="s">
@@ -44330,7 +44330,7 @@
         <v>750</v>
       </c>
       <c r="B784" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="C784" s="0"/>
       <c r="D784" t="s">
@@ -44344,7 +44344,7 @@
         <v>750</v>
       </c>
       <c r="B785" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="C785" s="0"/>
       <c r="D785" t="s">
@@ -44389,10 +44389,10 @@
     </row>
     <row r="788">
       <c r="A788" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B788" t="s">
-        <v>1068</v>
+        <v>548</v>
       </c>
       <c r="C788" s="0"/>
       <c r="D788" t="s">
@@ -44407,10 +44407,10 @@
     </row>
     <row r="789">
       <c r="A789" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B789" t="s">
-        <v>548</v>
+        <v>1068</v>
       </c>
       <c r="C789" s="0"/>
       <c r="D789" t="s">
@@ -44482,7 +44482,7 @@
         <v>748</v>
       </c>
       <c r="B793" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C793" s="0"/>
       <c r="D793" t="s">
@@ -44500,7 +44500,7 @@
         <v>748</v>
       </c>
       <c r="B794" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C794" s="0"/>
       <c r="D794" t="s">
@@ -44971,10 +44971,10 @@
     </row>
     <row r="821">
       <c r="A821" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B821" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C821" s="0"/>
       <c r="D821" t="s">
@@ -44989,10 +44989,10 @@
     </row>
     <row r="822">
       <c r="A822" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B822" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C822" s="0"/>
       <c r="D822" t="s">
@@ -45216,7 +45216,7 @@
         <v>1181</v>
       </c>
       <c r="B835" t="s">
-        <v>1094</v>
+        <v>842</v>
       </c>
       <c r="C835" s="0"/>
       <c r="D835" t="s">
@@ -45234,7 +45234,7 @@
         <v>1181</v>
       </c>
       <c r="B836" t="s">
-        <v>842</v>
+        <v>1094</v>
       </c>
       <c r="C836" s="0"/>
       <c r="D836" t="s">
@@ -45298,7 +45298,7 @@
         <v>748</v>
       </c>
       <c r="B840" t="s">
-        <v>1257</v>
+        <v>1283</v>
       </c>
       <c r="C840" s="0"/>
       <c r="D840" t="s">
@@ -45312,7 +45312,7 @@
         <v>748</v>
       </c>
       <c r="B841" t="s">
-        <v>1283</v>
+        <v>1257</v>
       </c>
       <c r="C841" s="0"/>
       <c r="D841" t="s">
@@ -45339,10 +45339,10 @@
     </row>
     <row r="843">
       <c r="A843" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B843" t="s">
-        <v>1257</v>
+        <v>1286</v>
       </c>
       <c r="C843" s="0"/>
       <c r="D843" t="s">
@@ -45355,10 +45355,10 @@
     </row>
     <row r="844">
       <c r="A844" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B844" t="s">
-        <v>1286</v>
+        <v>1257</v>
       </c>
       <c r="C844" s="0"/>
       <c r="D844" t="s">
@@ -45490,7 +45490,7 @@
         <v>748</v>
       </c>
       <c r="B852" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C852" s="0"/>
       <c r="D852" t="s">
@@ -45504,7 +45504,7 @@
         <v>748</v>
       </c>
       <c r="B853" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C853" s="0"/>
       <c r="D853" t="s">
@@ -45620,7 +45620,7 @@
         <v>748</v>
       </c>
       <c r="B860" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C860" s="0"/>
       <c r="D860" t="s">
@@ -45638,7 +45638,7 @@
         <v>748</v>
       </c>
       <c r="B861" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C861" s="0"/>
       <c r="D861" t="s">
@@ -45813,10 +45813,10 @@
     </row>
     <row r="872">
       <c r="A872" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B872" t="s">
-        <v>973</v>
+        <v>262</v>
       </c>
       <c r="C872" s="0"/>
       <c r="D872" t="s">
@@ -45831,10 +45831,10 @@
     </row>
     <row r="873">
       <c r="A873" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B873" t="s">
-        <v>262</v>
+        <v>973</v>
       </c>
       <c r="C873" s="0"/>
       <c r="D873" t="s">
@@ -47311,10 +47311,10 @@
     </row>
     <row r="960">
       <c r="A960" t="s">
-        <v>1181</v>
+        <v>750</v>
       </c>
       <c r="B960" t="s">
-        <v>1111</v>
+        <v>1155</v>
       </c>
       <c r="C960" s="0"/>
       <c r="D960" t="s">
@@ -47329,10 +47329,10 @@
     </row>
     <row r="961">
       <c r="A961" t="s">
-        <v>750</v>
+        <v>1181</v>
       </c>
       <c r="B961" t="s">
-        <v>1155</v>
+        <v>1111</v>
       </c>
       <c r="C961" s="0"/>
       <c r="D961" t="s">
@@ -47617,10 +47617,10 @@
     </row>
     <row r="978">
       <c r="A978" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="B978" t="s">
-        <v>1164</v>
+        <v>278</v>
       </c>
       <c r="C978" s="0"/>
       <c r="D978" t="s">
@@ -47635,10 +47635,10 @@
     </row>
     <row r="979">
       <c r="A979" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B979" t="s">
-        <v>278</v>
+        <v>1164</v>
       </c>
       <c r="C979" s="0"/>
       <c r="D979" t="s">
@@ -48056,7 +48056,7 @@
         <v>750</v>
       </c>
       <c r="B1003" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="C1003" s="0"/>
       <c r="D1003" t="s">
@@ -48070,7 +48070,7 @@
         <v>750</v>
       </c>
       <c r="B1004" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="C1004" s="0"/>
       <c r="D1004" t="s">

</xml_diff>